<commit_message>
update 1GTF column headers, fix typo in help
</commit_message>
<xml_diff>
--- a/docs/transcript_distance_column_descriptions.xlsx
+++ b/docs/transcript_distance_column_descriptions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
   <si>
     <t xml:space="preserve">ColumnName</t>
   </si>
@@ -37,238 +37,220 @@
     <t xml:space="preserve">transcript_1</t>
   </si>
   <si>
-    <t xml:space="preserve">Transcript ID for transcript 1 (T1) – will have suffix at the end of the transcript ID that represents the transcriptome of origin (“d1” by default, or name provided)</t>
+    <t xml:space="preserve">Transcript ID for transcript 1 (T1)</t>
   </si>
   <si>
     <t xml:space="preserve">transcript_2</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Transcript ID for transcript 2 (T2)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> – will have suffix at the end of the transcript ID that represents the transcriptome of origin (“d2” by default, or name provided)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">num_junction_T1_only</t>
+    <t xml:space="preserve">Transcript ID for transcript 2 (T2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num_jxn_only_T1</t>
   </si>
   <si>
     <t xml:space="preserve">Number of junctions in transcript 1 only</t>
   </si>
   <si>
-    <t xml:space="preserve">num_junction_T2_only</t>
+    <t xml:space="preserve">num_jxn_only_T2</t>
   </si>
   <si>
     <t xml:space="preserve">Number of junctions in transcript 2 only</t>
   </si>
   <si>
-    <t xml:space="preserve">num_junction_shared</t>
+    <t xml:space="preserve">num_jxn_ovlp</t>
   </si>
   <si>
     <t xml:space="preserve">Number of junctions shared by transcript 1 and transcript 2</t>
   </si>
   <si>
-    <t xml:space="preserve">prop_junction_diff</t>
+    <t xml:space="preserve">prop_jxn_noOvlp</t>
   </si>
   <si>
     <t xml:space="preserve">Proportion of different junctions ((num_junction_T1_only + num_junction_T2_only)/(num_junction_T1_only + num_junction_T2_only + num_junction_shared))</t>
   </si>
   <si>
-    <t xml:space="preserve">prop_junction_similar</t>
+    <t xml:space="preserve">prop_jxn_ovlp</t>
   </si>
   <si>
     <t xml:space="preserve">Proportion of shared junctions (num_junction_shared/(num_junction_T1_only + num_junction_T2_only + num_junction_shared))</t>
   </si>
   <si>
-    <t xml:space="preserve">junction_T1_only</t>
+    <t xml:space="preserve">jxn_string_T1</t>
   </si>
   <si>
     <t xml:space="preserve">Piped ("|") list of junction IDs (chr:start:end:strand) in transcript 1 only</t>
   </si>
   <si>
-    <t xml:space="preserve">junction_T2_only</t>
+    <t xml:space="preserve">jxn_string_T2</t>
   </si>
   <si>
     <t xml:space="preserve">Piped ("|") list of junction IDs (chr:start:end:strand) in transcript 2 only</t>
   </si>
   <si>
-    <t xml:space="preserve">junction_shared</t>
+    <t xml:space="preserve">jxn_same</t>
   </si>
   <si>
     <t xml:space="preserve">Piped ("|") list of junction IDs (chr:start:end:strand) shared by transcript 1 and transcript 2</t>
   </si>
   <si>
-    <t xml:space="preserve">num_ER_T1_only</t>
+    <t xml:space="preserve">num_ER_only_T1</t>
   </si>
   <si>
     <t xml:space="preserve">Number of exon regions in transcript 1 only</t>
   </si>
   <si>
-    <t xml:space="preserve">num_ER_T2_only</t>
+    <t xml:space="preserve">num_ER_only_T2</t>
   </si>
   <si>
     <t xml:space="preserve">Number of exon regions in transcript 2 only</t>
   </si>
   <si>
-    <t xml:space="preserve">num_ER_shared</t>
+    <t xml:space="preserve">num_ER_ovlp</t>
   </si>
   <si>
     <t xml:space="preserve">Number of exon regions shared by transcript 1 and transcript 2</t>
   </si>
   <si>
-    <t xml:space="preserve">prop_ER_diff</t>
+    <t xml:space="preserve">prop_ER_noOvlp</t>
   </si>
   <si>
     <t xml:space="preserve">Proportion of different exon regions ((num_ER_T1_only + num_ER_T2_only)/(num_ER_T1_only + num_ER_T2_only + num_ER_shared))</t>
   </si>
   <si>
-    <t xml:space="preserve">prop_ER_similar</t>
+    <t xml:space="preserve">prop_ER_ovlp</t>
   </si>
   <si>
     <t xml:space="preserve">Proportion of shared exon regions (num_ER_shared/(num_ER_T1_only + num_ER_T2_only + num_ER_shared))</t>
   </si>
   <si>
-    <t xml:space="preserve">ER_T1_only</t>
+    <t xml:space="preserve">ER_only_T1</t>
   </si>
   <si>
     <t xml:space="preserve">Piped ("|") list of exon region IDs in transcript 1 only</t>
   </si>
   <si>
-    <t xml:space="preserve">ER_T2_only</t>
+    <t xml:space="preserve">ER_only_T2</t>
   </si>
   <si>
     <t xml:space="preserve">Piped ("|") list of exon region IDs in transcript 2 only</t>
   </si>
   <si>
-    <t xml:space="preserve">ER_shared</t>
+    <t xml:space="preserve">ER_ovlp</t>
   </si>
   <si>
     <t xml:space="preserve">Piped ("|") list of exon region IDs shared by transcript 1 and transcript 2</t>
   </si>
   <si>
-    <t xml:space="preserve">num_fragment_T1_only</t>
+    <t xml:space="preserve">num_EF_only_T1</t>
   </si>
   <si>
     <t xml:space="preserve">Number of exon fragments in transcript 1 only</t>
   </si>
   <si>
-    <t xml:space="preserve">num_fragment_T2_only</t>
+    <t xml:space="preserve">num_EF_only_T2</t>
   </si>
   <si>
     <t xml:space="preserve">Number of exon fragments in transcript 2 only</t>
   </si>
   <si>
-    <t xml:space="preserve">num_fragment_shared</t>
+    <t xml:space="preserve">num_EF_ovlp</t>
   </si>
   <si>
     <t xml:space="preserve">Number of exon fragments shared by transcript 1 and transcript 2</t>
   </si>
   <si>
-    <t xml:space="preserve">prop_fragment_diff</t>
+    <t xml:space="preserve">prop_EF_noOvlp</t>
   </si>
   <si>
     <t xml:space="preserve">Proportion of different exon fragments ((num_fragment_T1_only + num_fragment_T2_only)/(num_fragment_T1_only + num_fragment_T2_only + num_fragment_shared))</t>
   </si>
   <si>
-    <t xml:space="preserve">prop_fragment_similar</t>
+    <t xml:space="preserve">prop_EF_ovlp</t>
   </si>
   <si>
     <t xml:space="preserve">Proportion of shared exon regions (num_fragment_shared/(num_fragment_T1_only + num_fragment_T2_only + num_fragment_shared))</t>
   </si>
   <si>
-    <t xml:space="preserve">fragment_T1_only</t>
+    <t xml:space="preserve">EF_only_T1</t>
   </si>
   <si>
     <t xml:space="preserve">Piped ("|") list of exon fragment IDs in transcript 1 only</t>
   </si>
   <si>
-    <t xml:space="preserve">fragment_T2_only</t>
+    <t xml:space="preserve">EF_only_T2</t>
   </si>
   <si>
     <t xml:space="preserve">Piped ("|") list of exon fragment IDs in transcript 2 only</t>
   </si>
   <si>
-    <t xml:space="preserve">fragment_shared</t>
+    <t xml:space="preserve">EF_ovlp</t>
   </si>
   <si>
     <t xml:space="preserve">Piped ("|") list of exon fragment IDs shared by transcript 1 and transcript 2</t>
   </si>
   <si>
-    <t xml:space="preserve">num_fragment_singletons_T1_only</t>
+    <t xml:space="preserve">num_exon_only_T1</t>
   </si>
   <si>
     <t xml:space="preserve">Number of exon fragment singletons (fragment is a full exon region) in transcript 1 only</t>
   </si>
   <si>
-    <t xml:space="preserve">num_fragment_singletons_T2_only</t>
+    <t xml:space="preserve">num_exon_only_T2</t>
   </si>
   <si>
     <t xml:space="preserve">Number of exon fragment singletons (fragment is a full exon region) in transcript 2 only</t>
   </si>
   <si>
-    <t xml:space="preserve">num_fragment_singletons_shared</t>
+    <t xml:space="preserve">num_exon_ovlp</t>
   </si>
   <si>
     <t xml:space="preserve">Number of exon fragment singletons (fragment is a full exon region) shared by transcript 1 and transcript 2</t>
   </si>
   <si>
-    <t xml:space="preserve">num_IR_T1</t>
+    <t xml:space="preserve">num_IR_EF_T1</t>
   </si>
   <si>
     <t xml:space="preserve">Number of intron retention events in transcript 1 (where an intron of transcript 2 is entirely contained within an exon of transcript 2)</t>
   </si>
   <si>
-    <t xml:space="preserve">num_IR_T2</t>
+    <t xml:space="preserve">num_IR_EF_T2</t>
   </si>
   <si>
     <t xml:space="preserve">Number of intron retention events in transcript 2 (where an intron of transcript 1 is entirely contained within an exon of transcript 2)</t>
   </si>
   <si>
-    <t xml:space="preserve">IR_T1</t>
+    <t xml:space="preserve">IR_EF_T1</t>
   </si>
   <si>
     <t xml:space="preserve">Piped ("|") list of intron IDs (chr:start:end:strand) retained in transcript 1</t>
   </si>
   <si>
-    <t xml:space="preserve">IR_T2</t>
+    <t xml:space="preserve">IR_EF_T2</t>
   </si>
   <si>
     <t xml:space="preserve">Piped ("|") list of intron IDs (chr:start:end:strand) retained in transcript 2</t>
   </si>
   <si>
-    <t xml:space="preserve">num_nt_T1_only</t>
+    <t xml:space="preserve">num_nt_ovlp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of nucleotides shared by transcript 1 and transcript 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num_nt_only_T1</t>
   </si>
   <si>
     <t xml:space="preserve">Number of nucleotides in transcript 1 only</t>
   </si>
   <si>
-    <t xml:space="preserve">num_nt_T2_only</t>
+    <t xml:space="preserve">num_nt_only_T2</t>
   </si>
   <si>
     <t xml:space="preserve">Number of nucleotides in transcript 2 only</t>
   </si>
   <si>
-    <t xml:space="preserve">num_nt_shared</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of nucleotides shared by transcript 1 and transcript 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">num_nt_diff</t>
+    <t xml:space="preserve">num_nt_noOvlp</t>
   </si>
   <si>
     <t xml:space="preserve">Number of nucleotides in only transcript 1 or only transcript 2</t>
@@ -280,61 +262,61 @@
     <t xml:space="preserve">Total number of nucleotides covered by either transcript 1 or transcript 2 (union)</t>
   </si>
   <si>
-    <t xml:space="preserve">prop_nt_diff</t>
+    <t xml:space="preserve">prop_nt_noOvlp</t>
   </si>
   <si>
     <t xml:space="preserve">Proportion of different nucleotides ((num_nt_T1_only + num_nt_T2_only)/total_nt)</t>
   </si>
   <si>
-    <t xml:space="preserve">prop_nt_similar</t>
+    <t xml:space="preserve">prop_nt_ovlp</t>
   </si>
   <si>
     <t xml:space="preserve">Proportion of shared nucleotides (num_nt_shared/total_nt)</t>
   </si>
   <si>
-    <t xml:space="preserve">num_nt_T1_only_in_shared_ER</t>
+    <t xml:space="preserve">num_nt_only_T1_in_ovlpER</t>
   </si>
   <si>
     <t xml:space="preserve">Number of nucleotides in transcript 1 only in shared exon regions, representing the number of nucelotides involved in IR (if present) and alt. donor/acceptors in transcript 1</t>
   </si>
   <si>
-    <t xml:space="preserve">num_nt_T2_only_in_shared_ER</t>
+    <t xml:space="preserve">num_nt_only_T2_in_ovlpER</t>
   </si>
   <si>
     <t xml:space="preserve">Number of nucleotides in transcript 2 only in shared exon regions, representing the number of nucelotides involved in IR (if present) and alt. donor/acceptors in transcript 2</t>
   </si>
   <si>
-    <t xml:space="preserve">num_nt_shared_in_shared_ER</t>
+    <t xml:space="preserve">num_nt_ovlp_in_ovlpER</t>
   </si>
   <si>
     <t xml:space="preserve">Number of nucleotides shared by transcript 1 and transcript 2 in shared exon regions</t>
   </si>
   <si>
-    <t xml:space="preserve">total_nt_in_shared_ER</t>
+    <t xml:space="preserve">total_nt_in_ovlpER</t>
   </si>
   <si>
     <t xml:space="preserve">Total number of nucleotides in shared exon regions</t>
   </si>
   <si>
-    <t xml:space="preserve">prop_nt_diff_in_shared_ER</t>
+    <t xml:space="preserve">prop_nt_noOvlp_in_ovlpER</t>
   </si>
   <si>
     <t xml:space="preserve">Proportion of different nucleotides in shared exon regions ((num_nt_T1_only_shared_ER + num_nt_T2_only_shared_ER)/total_nt_in_shared_ER)</t>
   </si>
   <si>
-    <t xml:space="preserve">prop_nt_similar_in_shared_ER</t>
+    <t xml:space="preserve">prop_nt_ovlp_in_ovlpER</t>
   </si>
   <si>
     <t xml:space="preserve">Proportion of shared nucleotides in shared exon regions (num_nt_shared_in_shared_ER/total_nt_in_shared_ER)</t>
   </si>
   <si>
-    <t xml:space="preserve">num_nt_T1_only_in_unique_ER</t>
+    <t xml:space="preserve">num_nt_only_T1_in_uniqER</t>
   </si>
   <si>
     <t xml:space="preserve">Number of nucleotides in transcript 1 only in exon regions unique to transcript 1</t>
   </si>
   <si>
-    <t xml:space="preserve">num_nt_T2_only_in_unique_ER</t>
+    <t xml:space="preserve">num_nt_only_T2_in_uniqER</t>
   </si>
   <si>
     <t xml:space="preserve">Number of nucleotides in transcript 2 only in exon regions unique to transcript 2</t>
@@ -346,25 +328,37 @@
     <t xml:space="preserve">Binary indicator (1,0) if transcript 1 and transcript 2 are full splice matches (FSM) of each other, meaning they share all the same junctions (prop_junction_diff == 0)</t>
   </si>
   <si>
+    <t xml:space="preserve">flag_T1_ISM_of_T2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Binary indicator (1,0) if transcript 1 is an incomplete splice match of transcript 2, meaning that transcript 1’s set of junctions is a complete consecutive subset of transcript 2’s. (flag is 0 if transcripts are FSM or either transcripts are a monoexon).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flag_T2_ISM_of_T1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Binary indicator (1,0) if transcript 2 is an incomplete splice match of transcript 1, meaning that transcript 2’s set of junctions is a complete consecutive subset of transcript 1’s. (flag is 0 if transcripts are FSM or either transcripts are a monoexon).</t>
+  </si>
+  <si>
     <t xml:space="preserve">flag_IR</t>
   </si>
   <si>
     <t xml:space="preserve">Binary indicator (1,0) if there is an intron retention event in the pair (num_IR_T1 + num_IR_T2 &gt; 0)</t>
   </si>
   <si>
-    <t xml:space="preserve">flag_5_variation</t>
+    <t xml:space="preserve">flag_5_var</t>
   </si>
   <si>
     <t xml:space="preserve">Binary indicator (1,0) if there is 5’ end (or TSS) variation in the pair (starts of transcripts are not the same)</t>
   </si>
   <si>
-    <t xml:space="preserve">flag_3_variation</t>
+    <t xml:space="preserve">flag_3_var</t>
   </si>
   <si>
     <t xml:space="preserve">Binary indicator (1,0) if there is 3’ end (or TTS) variation in the pair (ends of transcripts are not the same)</t>
   </si>
   <si>
-    <t xml:space="preserve">flag_alt_donor_acceptor</t>
+    <t xml:space="preserve">flag_alt_DA</t>
   </si>
   <si>
     <t xml:space="preserve">Binary indicator (1,0) if there is an alternate donor and/or alternate acceptor in the pair (num_nt_T1_only_in_shared_ER + num_nt_T2_only_in_shared_ER &gt; 0)</t>
@@ -376,7 +370,7 @@
     <t xml:space="preserve">Binary indicator (1,0) if there is an alternate exon in the pair (unique exon region in either transcript)</t>
   </si>
   <si>
-    <t xml:space="preserve">flag_no_shared_nt</t>
+    <t xml:space="preserve">flag_no_ovlp_nt</t>
   </si>
   <si>
     <t xml:space="preserve">Binary indicator (1,0) if the coordinates of the transcript pair do not overlap and therefore they do have any nucleotides in common</t>
@@ -422,15 +416,15 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -475,7 +469,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -496,8 +490,12 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -521,13 +519,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B58"/>
+  <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B63" activeCellId="0" sqref="B63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.89"/>
@@ -549,7 +547,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -557,7 +555,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -565,7 +563,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -573,7 +571,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -581,7 +579,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -589,7 +587,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="57.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
@@ -597,7 +595,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -605,7 +603,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -613,7 +611,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
@@ -621,7 +619,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
@@ -629,7 +627,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
         <v>24</v>
       </c>
@@ -637,7 +635,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
@@ -645,7 +643,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
         <v>28</v>
       </c>
@@ -653,7 +651,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="57.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
         <v>30</v>
       </c>
@@ -661,7 +659,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
         <v>32</v>
       </c>
@@ -669,7 +667,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
         <v>34</v>
       </c>
@@ -677,7 +675,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
         <v>36</v>
       </c>
@@ -685,7 +683,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
         <v>38</v>
       </c>
@@ -693,7 +691,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
         <v>40</v>
       </c>
@@ -701,7 +699,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
         <v>42</v>
       </c>
@@ -709,7 +707,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
         <v>44</v>
       </c>
@@ -717,7 +715,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="57.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
         <v>46</v>
       </c>
@@ -725,7 +723,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
         <v>48</v>
       </c>
@@ -733,7 +731,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
         <v>50</v>
       </c>
@@ -741,7 +739,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
         <v>52</v>
       </c>
@@ -749,7 +747,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
         <v>54</v>
       </c>
@@ -757,7 +755,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
         <v>56</v>
       </c>
@@ -765,7 +763,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
         <v>58</v>
       </c>
@@ -773,7 +771,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
         <v>60</v>
       </c>
@@ -781,7 +779,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
         <v>62</v>
       </c>
@@ -789,7 +787,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="s">
         <v>64</v>
       </c>
@@ -797,7 +795,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
         <v>66</v>
       </c>
@@ -805,7 +803,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
         <v>68</v>
       </c>
@@ -813,7 +811,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
         <v>70</v>
       </c>
@@ -821,7 +819,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
         <v>72</v>
       </c>
@@ -829,7 +827,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
         <v>74</v>
       </c>
@@ -853,7 +851,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
         <v>80</v>
       </c>
@@ -861,7 +859,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
         <v>82</v>
       </c>
@@ -885,7 +883,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
         <v>88</v>
       </c>
@@ -893,7 +891,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
         <v>90</v>
       </c>
@@ -917,7 +915,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
         <v>96</v>
       </c>
@@ -925,7 +923,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
         <v>98</v>
       </c>
@@ -941,23 +939,23 @@
         <v>101</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="5" t="s">
+    <row r="52" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="B52" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="5" t="s">
+    <row r="53" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="B53" s="7" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="5" t="s">
         <v>106</v>
       </c>
@@ -965,7 +963,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="5" t="s">
         <v>108</v>
       </c>
@@ -973,7 +971,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="5" t="s">
         <v>110</v>
       </c>
@@ -981,15 +979,31 @@
         <v>111</v>
       </c>
     </row>
-    <row r="57" s="4" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="4" t="s">
+    <row r="57" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="6" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" s="4" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>